<commit_message>
Deploying to gh-pages from  @ 089cbaa2e38d029f18c5c31973c074655159f8f7 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/3.9.1.1.xlsx
+++ b/en/downloads/data-excel/3.9.1.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="46">
   <si>
     <t>-</t>
   </si>
@@ -733,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -746,7 +746,7 @@
     <col min="5" max="5" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="39.75" customHeight="1">
+    <row r="1" spans="1:18" ht="39.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -770,7 +770,7 @@
       <c r="O1" s="11"/>
       <c r="P1" s="11"/>
     </row>
-    <row r="2" spans="1:17" ht="17.25" customHeight="1">
+    <row r="2" spans="1:18" ht="17.25" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
@@ -794,7 +794,7 @@
       <c r="O2" s="12"/>
       <c r="P2" s="12"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
+    <row r="3" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -812,7 +812,7 @@
       <c r="O3" s="12"/>
       <c r="P3" s="12"/>
     </row>
-    <row r="4" spans="1:17" s="3" customFormat="1" ht="18" customHeight="1" thickBot="1">
+    <row r="4" spans="1:18" s="3" customFormat="1" ht="18" customHeight="1" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -864,8 +864,11 @@
       <c r="Q4" s="8">
         <v>2020</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R4" s="8">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A5" s="14" t="s">
         <v>14</v>
       </c>
@@ -917,8 +920,11 @@
       <c r="Q5" s="33">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R5" s="33">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="19" t="s">
         <v>35</v>
       </c>
@@ -970,8 +976,11 @@
       <c r="Q6" s="34">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R6" s="34">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="19" t="s">
         <v>36</v>
       </c>
@@ -1023,8 +1032,11 @@
       <c r="Q7" s="34">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R7" s="34">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A8" s="19" t="s">
         <v>16</v>
       </c>
@@ -1076,8 +1088,11 @@
       <c r="Q8" s="35">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R8" s="35">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A9" s="19" t="s">
         <v>35</v>
       </c>
@@ -1129,8 +1144,11 @@
       <c r="Q9" s="35">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R9" s="35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A10" s="19" t="s">
         <v>36</v>
       </c>
@@ -1182,8 +1200,11 @@
       <c r="Q10" s="35">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R10" s="35">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>18</v>
       </c>
@@ -1235,8 +1256,11 @@
       <c r="Q11" s="35">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R11" s="35">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="19" t="s">
         <v>35</v>
       </c>
@@ -1288,8 +1312,11 @@
       <c r="Q12" s="35">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R12" s="35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A13" s="19" t="s">
         <v>36</v>
       </c>
@@ -1341,8 +1368,11 @@
       <c r="Q13" s="35">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R13" s="35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A14" s="19" t="s">
         <v>19</v>
       </c>
@@ -1394,8 +1424,11 @@
       <c r="Q14" s="35">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R14" s="35">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="19" t="s">
         <v>35</v>
       </c>
@@ -1447,8 +1480,11 @@
       <c r="Q15" s="35">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R15" s="35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="19" t="s">
         <v>36</v>
       </c>
@@ -1500,8 +1536,11 @@
       <c r="Q16" s="35">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R16" s="35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A17" s="19" t="s">
         <v>20</v>
       </c>
@@ -1553,8 +1592,11 @@
       <c r="Q17" s="35" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R17" s="35">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A18" s="19" t="s">
         <v>35</v>
       </c>
@@ -1606,8 +1648,11 @@
       <c r="Q18" s="35" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R18" s="35">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A19" s="19" t="s">
         <v>36</v>
       </c>
@@ -1659,8 +1704,11 @@
       <c r="Q19" s="35" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R19" s="35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A20" s="19" t="s">
         <v>22</v>
       </c>
@@ -1712,8 +1760,11 @@
       <c r="Q20" s="35">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R20" s="35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A21" s="19" t="s">
         <v>35</v>
       </c>
@@ -1765,8 +1816,11 @@
       <c r="Q21" s="35">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R21" s="35">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A22" s="19" t="s">
         <v>36</v>
       </c>
@@ -1818,8 +1872,11 @@
       <c r="Q22" s="35">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R22" s="35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A23" s="19" t="s">
         <v>24</v>
       </c>
@@ -1871,8 +1928,11 @@
       <c r="Q23" s="35" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R23" s="35">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A24" s="19" t="s">
         <v>35</v>
       </c>
@@ -1924,8 +1984,11 @@
       <c r="Q24" s="36" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R24" s="36">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A25" s="19" t="s">
         <v>36</v>
       </c>
@@ -1977,8 +2040,11 @@
       <c r="Q25" s="35" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R25" s="35">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A26" s="19" t="s">
         <v>26</v>
       </c>
@@ -2030,8 +2096,11 @@
       <c r="Q26" s="35">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R26" s="35">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A27" s="19" t="s">
         <v>35</v>
       </c>
@@ -2083,8 +2152,11 @@
       <c r="Q27" s="35">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R27" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A28" s="19" t="s">
         <v>36</v>
       </c>
@@ -2136,8 +2208,11 @@
       <c r="Q28" s="35">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R28" s="35">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A29" s="19" t="s">
         <v>28</v>
       </c>
@@ -2189,8 +2264,11 @@
       <c r="Q29" s="35">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R29" s="35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A30" s="19" t="s">
         <v>35</v>
       </c>
@@ -2242,8 +2320,11 @@
       <c r="Q30" s="35" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R30" s="35">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A31" s="19" t="s">
         <v>36</v>
       </c>
@@ -2295,8 +2376,11 @@
       <c r="Q31" s="35">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1">
+      <c r="R31" s="35">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1">
       <c r="A32" s="19" t="s">
         <v>31</v>
       </c>
@@ -2348,8 +2432,11 @@
       <c r="Q32" s="35">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="R32" s="35">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A33" s="19" t="s">
         <v>35</v>
       </c>
@@ -2401,8 +2488,11 @@
       <c r="Q33" s="35">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="R33" s="35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A34" s="26" t="s">
         <v>36</v>
       </c>
@@ -2453,6 +2543,9 @@
       </c>
       <c r="Q34" s="37" t="s">
         <v>0</v>
+      </c>
+      <c r="R34" s="37">
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>